<commit_message>
Parsing date from server and adding match percent
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8674CD74-E5E2-4280-A52A-2B0A62D9DA43}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
+    <workbookView xWindow="120" yWindow="108" windowWidth="15120" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <definedName name="ПрСмерти">'[1]Причина смерти'!$A$1:$A$7</definedName>
     <definedName name="Районы">[1]Районы!$A$1:$A$28</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -3203,8 +3204,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3283,11 +3284,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="AbsDb"/>
@@ -3538,7 +3547,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3570,9 +3579,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3604,6 +3631,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -3779,45 +3824,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC444"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="M418" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="V445" sqref="A11:V445"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="79.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="79.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" customWidth="1"/>
+    <col min="9" max="9" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" customWidth="1"/>
     <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="41.42578125" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" customWidth="1"/>
-    <col min="15" max="15" width="25.140625" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" customWidth="1"/>
+    <col min="13" max="13" width="41.44140625" customWidth="1"/>
+    <col min="14" max="14" width="21.44140625" customWidth="1"/>
+    <col min="15" max="15" width="25.109375" customWidth="1"/>
+    <col min="16" max="16" width="18.6640625" customWidth="1"/>
     <col min="17" max="17" width="21" customWidth="1"/>
-    <col min="18" max="18" width="12.5703125" customWidth="1"/>
-    <col min="19" max="19" width="19.140625" customWidth="1"/>
-    <col min="20" max="20" width="22.5703125" customWidth="1"/>
-    <col min="21" max="21" width="15.140625" customWidth="1"/>
+    <col min="18" max="18" width="12.5546875" customWidth="1"/>
+    <col min="19" max="19" width="19.109375" customWidth="1"/>
+    <col min="20" max="20" width="22.5546875" customWidth="1"/>
+    <col min="21" max="21" width="15.109375" customWidth="1"/>
     <col min="22" max="22" width="9" customWidth="1"/>
     <col min="23" max="29" width="0" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="6" customFormat="1">
+    <row r="1" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3906,7 +3951,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="6" customFormat="1">
+    <row r="2" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>134580</v>
       </c>
@@ -3970,7 +4015,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:29" s="6" customFormat="1">
+    <row r="3" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>134581</v>
       </c>
@@ -4036,7 +4081,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="4" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>134582</v>
       </c>
@@ -4104,7 +4149,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:29" s="6" customFormat="1">
+    <row r="5" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>134583</v>
       </c>
@@ -4170,7 +4215,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:29" s="6" customFormat="1">
+    <row r="6" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>134584</v>
       </c>
@@ -4236,7 +4281,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:29" s="6" customFormat="1">
+    <row r="7" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>134585</v>
       </c>
@@ -4302,7 +4347,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:29" s="6" customFormat="1">
+    <row r="8" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>134586</v>
       </c>
@@ -4368,7 +4413,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:29" s="6" customFormat="1">
+    <row r="9" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>134587</v>
       </c>
@@ -4434,7 +4479,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="10" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>134588</v>
       </c>
@@ -4504,7 +4549,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="11" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>134589</v>
       </c>
@@ -4572,7 +4617,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:29" s="6" customFormat="1">
+    <row r="12" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>134590</v>
       </c>
@@ -4638,7 +4683,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="13" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>134591</v>
       </c>
@@ -4708,7 +4753,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="14" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>134592</v>
       </c>
@@ -4778,7 +4823,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="15" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>134593</v>
       </c>
@@ -4848,7 +4893,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="16" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>134594</v>
       </c>
@@ -4914,7 +4959,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:29" s="6" customFormat="1">
+    <row r="17" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>145549</v>
       </c>
@@ -4978,7 +5023,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="18" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>134597</v>
       </c>
@@ -5046,7 +5091,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="19" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>134595</v>
       </c>
@@ -5112,7 +5157,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="20" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>134596</v>
       </c>
@@ -5182,7 +5227,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:29" s="6" customFormat="1">
+    <row r="21" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>134598</v>
       </c>
@@ -5248,7 +5293,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="22" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>134599</v>
       </c>
@@ -5316,7 +5361,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:29" s="6" customFormat="1">
+    <row r="23" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>134600</v>
       </c>
@@ -5378,7 +5423,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:29" s="6" customFormat="1">
+    <row r="24" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>134601</v>
       </c>
@@ -5442,7 +5487,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:29" s="6" customFormat="1">
+    <row r="25" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>134602</v>
       </c>
@@ -5508,7 +5553,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="1:29" s="6" customFormat="1">
+    <row r="26" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>134603</v>
       </c>
@@ -5572,7 +5617,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="27" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="27" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>134604</v>
       </c>
@@ -5638,7 +5683,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:29" s="6" customFormat="1">
+    <row r="28" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>134606</v>
       </c>
@@ -5706,7 +5751,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:29" s="6" customFormat="1">
+    <row r="29" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>134605</v>
       </c>
@@ -5772,7 +5817,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:29" s="6" customFormat="1">
+    <row r="30" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
         <v>134607</v>
       </c>
@@ -5838,7 +5883,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="31" spans="1:29" s="6" customFormat="1">
+    <row r="31" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <v>134608</v>
       </c>
@@ -5906,7 +5951,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="32" spans="1:29" s="6" customFormat="1">
+    <row r="32" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <v>134609</v>
       </c>
@@ -5974,7 +6019,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:29" s="6" customFormat="1">
+    <row r="33" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <v>134610</v>
       </c>
@@ -6038,7 +6083,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:29" s="6" customFormat="1">
+    <row r="34" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <v>134611</v>
       </c>
@@ -6102,7 +6147,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="1:29" s="6" customFormat="1">
+    <row r="35" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <v>134615</v>
       </c>
@@ -6168,7 +6213,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="36" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
         <v>134612</v>
       </c>
@@ -6234,7 +6279,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="37" spans="1:29" s="6" customFormat="1">
+    <row r="37" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7">
         <v>134613</v>
       </c>
@@ -6300,7 +6345,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="38" spans="1:29" s="6" customFormat="1">
+    <row r="38" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
         <v>134614</v>
       </c>
@@ -6366,7 +6411,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="39" spans="1:29" s="6" customFormat="1">
+    <row r="39" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <v>134616</v>
       </c>
@@ -6432,7 +6477,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="40" spans="1:29" s="6" customFormat="1">
+    <row r="40" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>134617</v>
       </c>
@@ -6496,7 +6541,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="41" spans="1:29" s="6" customFormat="1">
+    <row r="41" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>134618</v>
       </c>
@@ -6564,7 +6609,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="42" spans="1:29" s="6" customFormat="1">
+    <row r="42" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
         <v>134619</v>
       </c>
@@ -6628,7 +6673,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="43" spans="1:29" s="6" customFormat="1">
+    <row r="43" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <v>134620</v>
       </c>
@@ -6694,7 +6739,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="44" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="44" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A44" s="7">
         <v>134621</v>
       </c>
@@ -6764,7 +6809,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="45" spans="1:29" s="6" customFormat="1">
+    <row r="45" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
         <v>134622</v>
       </c>
@@ -6828,7 +6873,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="46" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="46" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A46" s="7">
         <v>134623</v>
       </c>
@@ -6898,7 +6943,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="47" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="47" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A47" s="7">
         <v>134624</v>
       </c>
@@ -6966,7 +7011,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="48" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="48" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A48" s="7">
         <v>134625</v>
       </c>
@@ -7030,7 +7075,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="49" spans="1:29" s="6" customFormat="1">
+    <row r="49" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7">
         <v>134626</v>
       </c>
@@ -7094,7 +7139,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="1:29" s="6" customFormat="1">
+    <row r="50" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7">
         <v>134627</v>
       </c>
@@ -7156,7 +7201,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="51" spans="1:29" s="6" customFormat="1">
+    <row r="51" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7">
         <v>134628</v>
       </c>
@@ -7220,7 +7265,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="52" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="52" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A52" s="7">
         <v>134629</v>
       </c>
@@ -7290,7 +7335,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="53" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="53" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A53" s="7">
         <v>145550</v>
       </c>
@@ -7358,7 +7403,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="54" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="54" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A54" s="7">
         <v>134630</v>
       </c>
@@ -7428,7 +7473,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="55" spans="1:29" s="6" customFormat="1">
+    <row r="55" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="7">
         <v>134632</v>
       </c>
@@ -7494,7 +7539,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="56" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="56" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A56" s="7">
         <v>134631</v>
       </c>
@@ -7562,7 +7607,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="57" spans="1:29" s="6" customFormat="1">
+    <row r="57" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="7">
         <v>134633</v>
       </c>
@@ -7630,7 +7675,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="58" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="58" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A58" s="7">
         <v>134634</v>
       </c>
@@ -7700,7 +7745,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="59" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="59" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A59" s="7">
         <v>134635</v>
       </c>
@@ -7770,7 +7815,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="60" spans="1:29" s="6" customFormat="1">
+    <row r="60" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="7">
         <v>134636</v>
       </c>
@@ -7836,7 +7881,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="61" spans="1:29" s="6" customFormat="1">
+    <row r="61" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
         <v>134637</v>
       </c>
@@ -7902,7 +7947,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="62" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="62" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A62" s="7">
         <v>134638</v>
       </c>
@@ -7972,7 +8017,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="63" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="63" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A63" s="7">
         <v>134639</v>
       </c>
@@ -8040,7 +8085,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="64" spans="1:29" s="6" customFormat="1">
+    <row r="64" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="7">
         <v>134640</v>
       </c>
@@ -8104,7 +8149,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="65" spans="1:29" s="6" customFormat="1">
+    <row r="65" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="7">
         <v>134641</v>
       </c>
@@ -8172,7 +8217,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="66" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="66" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A66" s="7">
         <v>134642</v>
       </c>
@@ -8238,7 +8283,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="67" spans="1:29" s="6" customFormat="1">
+    <row r="67" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="7">
         <v>134643</v>
       </c>
@@ -8304,7 +8349,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="68" spans="1:29" s="6" customFormat="1">
+    <row r="68" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="7">
         <v>134644</v>
       </c>
@@ -8372,7 +8417,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="69" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="69" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A69" s="7">
         <v>134645</v>
       </c>
@@ -8438,7 +8483,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="70" spans="1:29" s="6" customFormat="1">
+    <row r="70" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="7">
         <v>134646</v>
       </c>
@@ -8504,7 +8549,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="71" spans="1:29" s="6" customFormat="1">
+    <row r="71" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="7">
         <v>134647</v>
       </c>
@@ -8568,7 +8613,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="72" spans="1:29" s="6" customFormat="1">
+    <row r="72" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="7">
         <v>134649</v>
       </c>
@@ -8636,7 +8681,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="73" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="73" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A73" s="7">
         <v>134648</v>
       </c>
@@ -8706,7 +8751,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="74" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="74" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A74" s="7">
         <v>134650</v>
       </c>
@@ -8772,7 +8817,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="75" spans="1:29" s="6" customFormat="1">
+    <row r="75" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="7">
         <v>134651</v>
       </c>
@@ -8838,7 +8883,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="76" spans="1:29" s="6" customFormat="1">
+    <row r="76" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="7">
         <v>134652</v>
       </c>
@@ -8902,7 +8947,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="77" spans="1:29" s="6" customFormat="1">
+    <row r="77" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="7">
         <v>134653</v>
       </c>
@@ -8966,7 +9011,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="78" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="78" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A78" s="7">
         <v>134654</v>
       </c>
@@ -9032,7 +9077,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="79" spans="1:29" s="6" customFormat="1">
+    <row r="79" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="7">
         <v>134656</v>
       </c>
@@ -9098,7 +9143,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="80" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="80" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A80" s="7">
         <v>134655</v>
       </c>
@@ -9164,7 +9209,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="81" spans="1:29" s="6" customFormat="1">
+    <row r="81" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="7">
         <v>134657</v>
       </c>
@@ -9228,7 +9273,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="82" spans="1:29" s="6" customFormat="1">
+    <row r="82" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="7">
         <v>134658</v>
       </c>
@@ -9292,7 +9337,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="83" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="83" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A83" s="7">
         <v>134660</v>
       </c>
@@ -9356,7 +9401,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="84" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="84" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A84" s="7">
         <v>134661</v>
       </c>
@@ -9424,7 +9469,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="85" spans="1:29" s="6" customFormat="1">
+    <row r="85" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="7">
         <v>134659</v>
       </c>
@@ -9488,7 +9533,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="86" spans="1:29" s="6" customFormat="1">
+    <row r="86" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="7">
         <v>134662</v>
       </c>
@@ -9554,7 +9599,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="87" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="87" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A87" s="7">
         <v>134663</v>
       </c>
@@ -9624,7 +9669,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="88" spans="1:29" s="6" customFormat="1">
+    <row r="88" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="7">
         <v>134664</v>
       </c>
@@ -9688,7 +9733,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="89" spans="1:29" s="6" customFormat="1">
+    <row r="89" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="7">
         <v>134665</v>
       </c>
@@ -9754,7 +9799,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="90" spans="1:29" s="6" customFormat="1">
+    <row r="90" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="7">
         <v>134666</v>
       </c>
@@ -9818,7 +9863,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="91" spans="1:29" s="6" customFormat="1">
+    <row r="91" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="7">
         <v>134667</v>
       </c>
@@ -9884,7 +9929,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="92" spans="1:29" s="6" customFormat="1">
+    <row r="92" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="7">
         <v>134668</v>
       </c>
@@ -9948,7 +9993,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="93" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="93" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A93" s="7">
         <v>134669</v>
       </c>
@@ -10014,7 +10059,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="94" spans="1:29" s="6" customFormat="1">
+    <row r="94" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" s="7">
         <v>134670</v>
       </c>
@@ -10078,7 +10123,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="95" spans="1:29" s="6" customFormat="1">
+    <row r="95" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="7">
         <v>134671</v>
       </c>
@@ -10142,7 +10187,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="96" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="96" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A96" s="7">
         <v>134672</v>
       </c>
@@ -10210,7 +10255,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="97" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="97" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A97" s="7">
         <v>134674</v>
       </c>
@@ -10278,7 +10323,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="98" spans="1:29" s="6" customFormat="1">
+    <row r="98" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="7">
         <v>134675</v>
       </c>
@@ -10346,7 +10391,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="99" spans="1:29" s="6" customFormat="1">
+    <row r="99" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="7">
         <v>134676</v>
       </c>
@@ -10412,7 +10457,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="100" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="100" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A100" s="7">
         <v>134677</v>
       </c>
@@ -10482,7 +10527,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="101" spans="1:29" s="6" customFormat="1">
+    <row r="101" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="7">
         <v>134678</v>
       </c>
@@ -10548,7 +10593,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="102" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="102" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A102" s="7">
         <v>134679</v>
       </c>
@@ -10616,7 +10661,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="103" spans="1:29" s="6" customFormat="1">
+    <row r="103" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="7">
         <v>134680</v>
       </c>
@@ -10682,7 +10727,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="104" spans="1:29" s="6" customFormat="1">
+    <row r="104" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="7">
         <v>134681</v>
       </c>
@@ -10750,7 +10795,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="105" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="105" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A105" s="7">
         <v>134682</v>
       </c>
@@ -10818,7 +10863,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="106" spans="1:29" s="6" customFormat="1">
+    <row r="106" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="7">
         <v>134683</v>
       </c>
@@ -10882,7 +10927,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="107" spans="1:29" s="6" customFormat="1">
+    <row r="107" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="7">
         <v>134684</v>
       </c>
@@ -10948,7 +10993,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="108" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="108" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A108" s="7">
         <v>134685</v>
       </c>
@@ -11018,7 +11063,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="109" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="109" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A109" s="7">
         <v>134673</v>
       </c>
@@ -11086,7 +11131,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="110" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="110" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A110" s="7">
         <v>134686</v>
       </c>
@@ -11156,7 +11201,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="111" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="111" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A111" s="7">
         <v>134687</v>
       </c>
@@ -11226,7 +11271,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="112" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="112" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A112" s="7">
         <v>134688</v>
       </c>
@@ -11294,7 +11339,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="113" spans="1:29" s="6" customFormat="1">
+    <row r="113" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="7">
         <v>134689</v>
       </c>
@@ -11360,7 +11405,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="114" spans="1:29" s="6" customFormat="1">
+    <row r="114" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="7">
         <v>134691</v>
       </c>
@@ -11426,7 +11471,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="115" spans="1:29" s="6" customFormat="1">
+    <row r="115" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="7">
         <v>134690</v>
       </c>
@@ -11490,7 +11535,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="116" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="116" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="7">
         <v>134692</v>
       </c>
@@ -11556,7 +11601,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="117" spans="1:29" s="6" customFormat="1">
+    <row r="117" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="7">
         <v>134693</v>
       </c>
@@ -11624,7 +11669,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="118" spans="1:29" s="6" customFormat="1">
+    <row r="118" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="7">
         <v>134694</v>
       </c>
@@ -11692,7 +11737,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="119" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="119" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A119" s="7">
         <v>134695</v>
       </c>
@@ -11758,7 +11803,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="120" spans="1:29" s="6" customFormat="1">
+    <row r="120" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="7">
         <v>134696</v>
       </c>
@@ -11824,7 +11869,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="121" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="121" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A121" s="7">
         <v>134697</v>
       </c>
@@ -11890,7 +11935,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="122" spans="1:29" s="6" customFormat="1">
+    <row r="122" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="7">
         <v>134698</v>
       </c>
@@ -11956,7 +12001,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="123" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="123" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A123" s="7">
         <v>134699</v>
       </c>
@@ -12026,7 +12071,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="124" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="124" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A124" s="7">
         <v>134700</v>
       </c>
@@ -12094,7 +12139,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="125" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="125" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A125" s="7">
         <v>134701</v>
       </c>
@@ -12160,7 +12205,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="126" spans="1:29" s="6" customFormat="1">
+    <row r="126" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="7">
         <v>134702</v>
       </c>
@@ -12226,7 +12271,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="127" spans="1:29" s="6" customFormat="1">
+    <row r="127" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="7">
         <v>134703</v>
       </c>
@@ -12290,7 +12335,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="128" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="128" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A128" s="7">
         <v>134704</v>
       </c>
@@ -12358,7 +12403,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="129" spans="1:29" s="6" customFormat="1">
+    <row r="129" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="7">
         <v>134705</v>
       </c>
@@ -12424,7 +12469,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="130" spans="1:29" s="6" customFormat="1">
+    <row r="130" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="7">
         <v>134706</v>
       </c>
@@ -12488,7 +12533,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="131" spans="1:29" s="6" customFormat="1">
+    <row r="131" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="7">
         <v>134710</v>
       </c>
@@ -12552,7 +12597,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="132" spans="1:29" s="6" customFormat="1">
+    <row r="132" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="7">
         <v>134707</v>
       </c>
@@ -12618,7 +12663,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="133" spans="1:29" s="6" customFormat="1">
+    <row r="133" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="7">
         <v>134709</v>
       </c>
@@ -12686,7 +12731,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="134" spans="1:29" s="6" customFormat="1">
+    <row r="134" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="7">
         <v>134708</v>
       </c>
@@ -12750,7 +12795,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="135" spans="1:29" s="6" customFormat="1">
+    <row r="135" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="7">
         <v>134711</v>
       </c>
@@ -12814,7 +12859,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="136" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="136" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A136" s="7">
         <v>134712</v>
       </c>
@@ -12884,7 +12929,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="137" spans="1:29" s="6" customFormat="1">
+    <row r="137" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="7">
         <v>134714</v>
       </c>
@@ -12950,7 +12995,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="138" spans="1:29" s="6" customFormat="1">
+    <row r="138" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="7">
         <v>134713</v>
       </c>
@@ -13014,7 +13059,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="139" spans="1:29" s="6" customFormat="1">
+    <row r="139" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="7">
         <v>134715</v>
       </c>
@@ -13078,7 +13123,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="140" spans="1:29" s="6" customFormat="1">
+    <row r="140" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="7">
         <v>134716</v>
       </c>
@@ -13144,7 +13189,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="141" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="141" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A141" s="7">
         <v>134717</v>
       </c>
@@ -13212,7 +13257,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="142" spans="1:29" s="6" customFormat="1">
+    <row r="142" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="7">
         <v>134718</v>
       </c>
@@ -13276,7 +13321,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="143" spans="1:29" s="6" customFormat="1">
+    <row r="143" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="7">
         <v>134719</v>
       </c>
@@ -13340,7 +13385,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="144" spans="1:29" s="6" customFormat="1">
+    <row r="144" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="7">
         <v>134720</v>
       </c>
@@ -13406,7 +13451,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="145" spans="1:29" s="6" customFormat="1">
+    <row r="145" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="7">
         <v>134721</v>
       </c>
@@ -13472,7 +13517,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="146" spans="1:29" s="6" customFormat="1" ht="39">
+    <row r="146" spans="1:29" s="6" customFormat="1" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A146" s="7">
         <v>134722</v>
       </c>
@@ -13542,7 +13587,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="147" spans="1:29" s="6" customFormat="1">
+    <row r="147" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="7">
         <v>134723</v>
       </c>
@@ -13606,7 +13651,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="148" spans="1:29" s="6" customFormat="1">
+    <row r="148" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A148" s="7">
         <v>134724</v>
       </c>
@@ -13670,7 +13715,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="149" spans="1:29" s="6" customFormat="1">
+    <row r="149" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A149" s="7">
         <v>134725</v>
       </c>
@@ -13734,7 +13779,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="150" spans="1:29" s="6" customFormat="1">
+    <row r="150" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A150" s="7">
         <v>134726</v>
       </c>
@@ -13802,7 +13847,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="151" spans="1:29" s="6" customFormat="1">
+    <row r="151" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A151" s="7">
         <v>134727</v>
       </c>
@@ -13866,7 +13911,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="152" spans="1:29" s="6" customFormat="1">
+    <row r="152" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A152" s="7">
         <v>134728</v>
       </c>
@@ -13930,7 +13975,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="153" spans="1:29" s="6" customFormat="1">
+    <row r="153" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A153" s="7">
         <v>134729</v>
       </c>
@@ -13994,7 +14039,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="154" spans="1:29" s="6" customFormat="1">
+    <row r="154" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A154" s="7">
         <v>145551</v>
       </c>
@@ -14058,7 +14103,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="155" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="155" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A155" s="7">
         <v>145552</v>
       </c>
@@ -14128,7 +14173,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="156" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="156" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A156" s="7">
         <v>134730</v>
       </c>
@@ -14198,7 +14243,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="157" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="157" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A157" s="7">
         <v>134731</v>
       </c>
@@ -14266,7 +14311,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="158" spans="1:29" s="6" customFormat="1">
+    <row r="158" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A158" s="7">
         <v>134732</v>
       </c>
@@ -14332,7 +14377,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="159" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="159" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A159" s="7">
         <v>134733</v>
       </c>
@@ -14400,7 +14445,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="160" spans="1:29" s="6" customFormat="1">
+    <row r="160" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A160" s="7">
         <v>134734</v>
       </c>
@@ -14464,7 +14509,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="161" spans="1:29" s="6" customFormat="1">
+    <row r="161" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A161" s="7">
         <v>134735</v>
       </c>
@@ -14530,7 +14575,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="162" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="162" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A162" s="7">
         <v>134736</v>
       </c>
@@ -14598,7 +14643,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="163" spans="1:29" s="6" customFormat="1">
+    <row r="163" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A163" s="7">
         <v>134737</v>
       </c>
@@ -14666,7 +14711,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="164" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="164" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A164" s="7">
         <v>134738</v>
       </c>
@@ -14732,7 +14777,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="165" spans="1:29" s="6" customFormat="1">
+    <row r="165" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A165" s="7">
         <v>134739</v>
       </c>
@@ -14798,7 +14843,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="166" spans="1:29" s="6" customFormat="1">
+    <row r="166" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A166" s="7">
         <v>134740</v>
       </c>
@@ -14862,7 +14907,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="167" spans="1:29" s="6" customFormat="1">
+    <row r="167" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A167" s="7">
         <v>134741</v>
       </c>
@@ -14926,7 +14971,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="168" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="168" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A168" s="7">
         <v>134742</v>
       </c>
@@ -14994,7 +15039,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="169" spans="1:29" s="6" customFormat="1">
+    <row r="169" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A169" s="7">
         <v>134743</v>
       </c>
@@ -15058,7 +15103,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="170" spans="1:29" s="6" customFormat="1">
+    <row r="170" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A170" s="7">
         <v>134744</v>
       </c>
@@ -15126,7 +15171,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="171" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="171" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A171" s="7">
         <v>134745</v>
       </c>
@@ -15192,7 +15237,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="172" spans="1:29" s="6" customFormat="1">
+    <row r="172" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A172" s="7">
         <v>134746</v>
       </c>
@@ -15256,7 +15301,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="173" spans="1:29" s="6" customFormat="1">
+    <row r="173" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A173" s="7">
         <v>134747</v>
       </c>
@@ -15324,7 +15369,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="174" spans="1:29" s="6" customFormat="1">
+    <row r="174" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A174" s="7">
         <v>134748</v>
       </c>
@@ -15390,7 +15435,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="175" spans="1:29" s="6" customFormat="1">
+    <row r="175" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A175" s="7">
         <v>134749</v>
       </c>
@@ -15456,7 +15501,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="176" spans="1:29" s="6" customFormat="1">
+    <row r="176" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A176" s="7">
         <v>134750</v>
       </c>
@@ -15520,7 +15565,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="177" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="177" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A177" s="7">
         <v>145553</v>
       </c>
@@ -15586,7 +15631,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="178" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="178" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A178" s="7">
         <v>134751</v>
       </c>
@@ -15656,7 +15701,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="179" spans="1:29" s="6" customFormat="1">
+    <row r="179" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A179" s="7">
         <v>134752</v>
       </c>
@@ -15722,7 +15767,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="180" spans="1:29" s="6" customFormat="1">
+    <row r="180" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A180" s="7">
         <v>134753</v>
       </c>
@@ -15788,7 +15833,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="181" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="181" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A181" s="7">
         <v>134754</v>
       </c>
@@ -15854,7 +15899,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="182" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="182" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A182" s="7">
         <v>134755</v>
       </c>
@@ -15924,7 +15969,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="183" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="183" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A183" s="7">
         <v>134756</v>
       </c>
@@ -15994,7 +16039,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="184" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="184" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A184" s="7">
         <v>134757</v>
       </c>
@@ -16062,7 +16107,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="185" spans="1:29" s="6" customFormat="1">
+    <row r="185" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A185" s="7">
         <v>134758</v>
       </c>
@@ -16130,7 +16175,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="186" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="186" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A186" s="7">
         <v>134759</v>
       </c>
@@ -16198,7 +16243,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="187" spans="1:29" s="6" customFormat="1">
+    <row r="187" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A187" s="7">
         <v>134760</v>
       </c>
@@ -16262,7 +16307,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="188" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="188" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A188" s="7">
         <v>134761</v>
       </c>
@@ -16332,7 +16377,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="189" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="189" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A189" s="7">
         <v>134762</v>
       </c>
@@ -16402,7 +16447,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="190" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="190" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A190" s="7">
         <v>134763</v>
       </c>
@@ -16472,7 +16517,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="191" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="191" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A191" s="7">
         <v>134764</v>
       </c>
@@ -16540,7 +16585,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="192" spans="1:29" s="6" customFormat="1">
+    <row r="192" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A192" s="7">
         <v>134765</v>
       </c>
@@ -16604,7 +16649,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="193" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="193" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A193" s="7">
         <v>145554</v>
       </c>
@@ -16674,7 +16719,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="194" spans="1:29" s="6" customFormat="1">
+    <row r="194" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A194" s="7">
         <v>134766</v>
       </c>
@@ -16738,7 +16783,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="195" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="195" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A195" s="7">
         <v>134767</v>
       </c>
@@ -16808,7 +16853,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="196" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="196" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A196" s="7">
         <v>134768</v>
       </c>
@@ -16878,7 +16923,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="197" spans="1:29" s="6" customFormat="1">
+    <row r="197" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A197" s="7">
         <v>134769</v>
       </c>
@@ -16946,7 +16991,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="198" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="198" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A198" s="7">
         <v>134770</v>
       </c>
@@ -17016,7 +17061,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="199" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="199" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A199" s="7">
         <v>134771</v>
       </c>
@@ -17084,7 +17129,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="200" spans="1:29" s="6" customFormat="1">
+    <row r="200" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A200" s="7">
         <v>134772</v>
       </c>
@@ -17150,7 +17195,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="201" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="201" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A201" s="7">
         <v>134773</v>
       </c>
@@ -17218,7 +17263,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="202" spans="1:29" s="6" customFormat="1">
+    <row r="202" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A202" s="7">
         <v>134774</v>
       </c>
@@ -17284,7 +17329,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="203" spans="1:29" s="6" customFormat="1">
+    <row r="203" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A203" s="7">
         <v>134775</v>
       </c>
@@ -17348,7 +17393,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="204" spans="1:29" s="6" customFormat="1">
+    <row r="204" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A204" s="7">
         <v>134776</v>
       </c>
@@ -17414,7 +17459,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="205" spans="1:29" s="6" customFormat="1">
+    <row r="205" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A205" s="7">
         <v>134777</v>
       </c>
@@ -17480,7 +17525,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="206" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="206" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A206" s="7">
         <v>134778</v>
       </c>
@@ -17548,7 +17593,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="207" spans="1:29" s="6" customFormat="1">
+    <row r="207" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A207" s="7">
         <v>134779</v>
       </c>
@@ -17614,7 +17659,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="208" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="208" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A208" s="7">
         <v>134780</v>
       </c>
@@ -17682,7 +17727,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="209" spans="1:29" s="6" customFormat="1">
+    <row r="209" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A209" s="7">
         <v>134781</v>
       </c>
@@ -17750,7 +17795,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="210" spans="1:29" s="6" customFormat="1">
+    <row r="210" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A210" s="7">
         <v>134782</v>
       </c>
@@ -17814,7 +17859,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="211" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="211" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A211" s="7">
         <v>134783</v>
       </c>
@@ -17882,7 +17927,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="212" spans="1:29" s="6" customFormat="1">
+    <row r="212" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A212" s="7">
         <v>134784</v>
       </c>
@@ -17948,7 +17993,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="213" spans="1:29" s="6" customFormat="1" ht="39">
+    <row r="213" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A213" s="7">
         <v>134785</v>
       </c>
@@ -18018,7 +18063,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="214" spans="1:29" s="6" customFormat="1">
+    <row r="214" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A214" s="7">
         <v>134786</v>
       </c>
@@ -18084,7 +18129,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="215" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="215" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A215" s="7">
         <v>134787</v>
       </c>
@@ -18152,7 +18197,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="216" spans="1:29" s="6" customFormat="1">
+    <row r="216" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A216" s="7">
         <v>134788</v>
       </c>
@@ -18220,7 +18265,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="217" spans="1:29" s="6" customFormat="1">
+    <row r="217" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A217" s="7">
         <v>134789</v>
       </c>
@@ -18288,7 +18333,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="218" spans="1:29" s="6" customFormat="1">
+    <row r="218" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A218" s="7">
         <v>134790</v>
       </c>
@@ -18352,7 +18397,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="219" spans="1:29" s="6" customFormat="1">
+    <row r="219" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A219" s="7">
         <v>134791</v>
       </c>
@@ -18416,7 +18461,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="220" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="220" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A220" s="7">
         <v>134792</v>
       </c>
@@ -18486,7 +18531,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="221" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="221" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A221" s="7">
         <v>134793</v>
       </c>
@@ -18556,7 +18601,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="222" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="222" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A222" s="7">
         <v>134794</v>
       </c>
@@ -18626,7 +18671,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="223" spans="1:29" s="6" customFormat="1">
+    <row r="223" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A223" s="7">
         <v>134795</v>
       </c>
@@ -18694,7 +18739,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="224" spans="1:29" s="6" customFormat="1">
+    <row r="224" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A224" s="7">
         <v>134796</v>
       </c>
@@ -18758,7 +18803,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="225" spans="1:29" s="6" customFormat="1">
+    <row r="225" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A225" s="7">
         <v>134797</v>
       </c>
@@ -18824,7 +18869,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="226" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="226" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A226" s="7">
         <v>134799</v>
       </c>
@@ -18892,7 +18937,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="227" spans="1:29" s="6" customFormat="1">
+    <row r="227" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A227" s="7">
         <v>134798</v>
       </c>
@@ -18960,7 +19005,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="228" spans="1:29" s="6" customFormat="1">
+    <row r="228" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A228" s="7">
         <v>134800</v>
       </c>
@@ -19026,7 +19071,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="229" spans="1:29" s="6" customFormat="1">
+    <row r="229" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A229" s="7">
         <v>134801</v>
       </c>
@@ -19088,7 +19133,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="230" spans="1:29" s="6" customFormat="1">
+    <row r="230" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A230" s="7">
         <v>134802</v>
       </c>
@@ -19154,7 +19199,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="231" spans="1:29" s="6" customFormat="1">
+    <row r="231" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A231" s="7">
         <v>134803</v>
       </c>
@@ -19218,7 +19263,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="232" spans="1:29" s="6" customFormat="1">
+    <row r="232" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A232" s="7">
         <v>145555</v>
       </c>
@@ -19282,7 +19327,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="233" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="233" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A233" s="7">
         <v>134804</v>
       </c>
@@ -19352,7 +19397,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="234" spans="1:29" s="6" customFormat="1">
+    <row r="234" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A234" s="7">
         <v>134805</v>
       </c>
@@ -19416,7 +19461,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="235" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="235" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A235" s="7">
         <v>134806</v>
       </c>
@@ -19484,7 +19529,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="236" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="236" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A236" s="7">
         <v>134807</v>
       </c>
@@ -19554,7 +19599,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="237" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="237" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A237" s="7">
         <v>134808</v>
       </c>
@@ -19624,7 +19669,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="238" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="238" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A238" s="7">
         <v>134809</v>
       </c>
@@ -19692,7 +19737,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="239" spans="1:29" s="6" customFormat="1">
+    <row r="239" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A239" s="7">
         <v>134810</v>
       </c>
@@ -19758,7 +19803,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="240" spans="1:29" s="6" customFormat="1">
+    <row r="240" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A240" s="7">
         <v>134811</v>
       </c>
@@ -19822,7 +19867,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="241" spans="1:29" s="6" customFormat="1">
+    <row r="241" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A241" s="7">
         <v>134814</v>
       </c>
@@ -19888,7 +19933,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="242" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="242" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A242" s="7">
         <v>134812</v>
       </c>
@@ -19956,7 +20001,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="243" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="243" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A243" s="7">
         <v>134813</v>
       </c>
@@ -20022,7 +20067,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="244" spans="1:29" s="6" customFormat="1">
+    <row r="244" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A244" s="7">
         <v>134815</v>
       </c>
@@ -20086,7 +20131,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="245" spans="1:29" s="6" customFormat="1">
+    <row r="245" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A245" s="7">
         <v>134816</v>
       </c>
@@ -20150,7 +20195,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="246" spans="1:29" s="6" customFormat="1">
+    <row r="246" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A246" s="7">
         <v>134817</v>
       </c>
@@ -20216,7 +20261,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="247" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="247" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A247" s="7">
         <v>134818</v>
       </c>
@@ -20286,7 +20331,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="248" spans="1:29" s="6" customFormat="1">
+    <row r="248" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A248" s="7">
         <v>134819</v>
       </c>
@@ -20354,7 +20399,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="249" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="249" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A249" s="7">
         <v>134820</v>
       </c>
@@ -20424,7 +20469,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="250" spans="1:29" s="6" customFormat="1">
+    <row r="250" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A250" s="7">
         <v>134821</v>
       </c>
@@ -20492,7 +20537,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="251" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="251" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A251" s="7">
         <v>134822</v>
       </c>
@@ -20560,7 +20605,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="252" spans="1:29" s="6" customFormat="1">
+    <row r="252" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A252" s="7">
         <v>134823</v>
       </c>
@@ -20624,7 +20669,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="253" spans="1:29" s="6" customFormat="1">
+    <row r="253" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A253" s="7">
         <v>134824</v>
       </c>
@@ -20688,7 +20733,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="254" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="254" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A254" s="7">
         <v>134825</v>
       </c>
@@ -20758,7 +20803,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="255" spans="1:29" s="6" customFormat="1">
+    <row r="255" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A255" s="7">
         <v>134826</v>
       </c>
@@ -20824,7 +20869,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="256" spans="1:29" s="6" customFormat="1">
+    <row r="256" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A256" s="7">
         <v>134827</v>
       </c>
@@ -20890,7 +20935,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="257" spans="1:29" s="6" customFormat="1">
+    <row r="257" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A257" s="7">
         <v>134828</v>
       </c>
@@ -20954,7 +20999,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="258" spans="1:29" s="6" customFormat="1">
+    <row r="258" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A258" s="7">
         <v>134829</v>
       </c>
@@ -21020,7 +21065,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="259" spans="1:29" s="6" customFormat="1">
+    <row r="259" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A259" s="7">
         <v>134830</v>
       </c>
@@ -21084,7 +21129,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="260" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="260" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A260" s="7">
         <v>134831</v>
       </c>
@@ -21154,7 +21199,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="261" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="261" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A261" s="7">
         <v>134832</v>
       </c>
@@ -21222,7 +21267,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="262" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="262" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A262" s="7">
         <v>134833</v>
       </c>
@@ -21292,7 +21337,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="263" spans="1:29" s="6" customFormat="1">
+    <row r="263" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A263" s="7">
         <v>145556</v>
       </c>
@@ -21358,7 +21403,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="264" spans="1:29" s="6" customFormat="1">
+    <row r="264" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A264" s="7">
         <v>145557</v>
       </c>
@@ -21424,7 +21469,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="265" spans="1:29" s="6" customFormat="1">
+    <row r="265" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A265" s="7">
         <v>134834</v>
       </c>
@@ -21490,7 +21535,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="266" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="266" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A266" s="7">
         <v>134835</v>
       </c>
@@ -21560,7 +21605,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="267" spans="1:29" s="6" customFormat="1">
+    <row r="267" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A267" s="7">
         <v>134836</v>
       </c>
@@ -21626,7 +21671,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="268" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="268" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A268" s="7">
         <v>134837</v>
       </c>
@@ -21696,7 +21741,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="269" spans="1:29" s="6" customFormat="1">
+    <row r="269" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A269" s="7">
         <v>134838</v>
       </c>
@@ -21764,7 +21809,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="270" spans="1:29" s="6" customFormat="1">
+    <row r="270" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A270" s="7">
         <v>134839</v>
       </c>
@@ -21828,7 +21873,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="271" spans="1:29" s="6" customFormat="1">
+    <row r="271" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A271" s="7">
         <v>134840</v>
       </c>
@@ -21892,7 +21937,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="272" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="272" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A272" s="7">
         <v>134841</v>
       </c>
@@ -21960,7 +22005,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="273" spans="1:29" s="6" customFormat="1">
+    <row r="273" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A273" s="7">
         <v>134842</v>
       </c>
@@ -22026,7 +22071,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="274" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="274" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A274" s="7">
         <v>134843</v>
       </c>
@@ -22096,7 +22141,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="275" spans="1:29" s="6" customFormat="1">
+    <row r="275" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A275" s="7">
         <v>134844</v>
       </c>
@@ -22160,7 +22205,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="276" spans="1:29" s="6" customFormat="1">
+    <row r="276" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A276" s="7">
         <v>134845</v>
       </c>
@@ -22226,7 +22271,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="277" spans="1:29" s="6" customFormat="1">
+    <row r="277" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A277" s="7">
         <v>134846</v>
       </c>
@@ -22292,7 +22337,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="278" spans="1:29" s="6" customFormat="1">
+    <row r="278" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A278" s="7">
         <v>134847</v>
       </c>
@@ -22358,7 +22403,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="279" spans="1:29" s="6" customFormat="1">
+    <row r="279" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A279" s="7">
         <v>134848</v>
       </c>
@@ -22424,7 +22469,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="280" spans="1:29" s="6" customFormat="1">
+    <row r="280" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A280" s="7">
         <v>134849</v>
       </c>
@@ -22492,7 +22537,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="281" spans="1:29" s="6" customFormat="1">
+    <row r="281" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A281" s="7">
         <v>134850</v>
       </c>
@@ -22556,7 +22601,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="282" spans="1:29" s="6" customFormat="1">
+    <row r="282" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A282" s="7">
         <v>134851</v>
       </c>
@@ -22622,7 +22667,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="283" spans="1:29" s="6" customFormat="1">
+    <row r="283" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A283" s="7">
         <v>134852</v>
       </c>
@@ -22690,7 +22735,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="284" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="284" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A284" s="7">
         <v>134853</v>
       </c>
@@ -22760,7 +22805,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="285" spans="1:29" s="6" customFormat="1">
+    <row r="285" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A285" s="7">
         <v>134854</v>
       </c>
@@ -22826,7 +22871,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="286" spans="1:29" s="6" customFormat="1">
+    <row r="286" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A286" s="7">
         <v>134855</v>
       </c>
@@ -22892,7 +22937,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="287" spans="1:29" s="6" customFormat="1">
+    <row r="287" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A287" s="7">
         <v>134856</v>
       </c>
@@ -22956,7 +23001,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="288" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="288" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A288" s="7">
         <v>134857</v>
       </c>
@@ -23026,7 +23071,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="289" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="289" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A289" s="7">
         <v>134858</v>
       </c>
@@ -23094,7 +23139,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="290" spans="1:29" s="6" customFormat="1">
+    <row r="290" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A290" s="7">
         <v>134859</v>
       </c>
@@ -23162,7 +23207,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="291" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="291" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A291" s="7">
         <v>134860</v>
       </c>
@@ -23228,7 +23273,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="292" spans="1:29" s="6" customFormat="1">
+    <row r="292" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A292" s="7">
         <v>134861</v>
       </c>
@@ -23292,7 +23337,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="293" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="293" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A293" s="7">
         <v>134862</v>
       </c>
@@ -23360,7 +23405,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="294" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="294" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A294" s="7">
         <v>134863</v>
       </c>
@@ -23430,7 +23475,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="295" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="295" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A295" s="7">
         <v>134864</v>
       </c>
@@ -23500,7 +23545,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="296" spans="1:29" s="6" customFormat="1">
+    <row r="296" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A296" s="7">
         <v>134865</v>
       </c>
@@ -23566,7 +23611,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="297" spans="1:29" s="6" customFormat="1">
+    <row r="297" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A297" s="7">
         <v>134866</v>
       </c>
@@ -23632,7 +23677,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="298" spans="1:29" s="6" customFormat="1">
+    <row r="298" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A298" s="7">
         <v>134867</v>
       </c>
@@ -23698,7 +23743,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="299" spans="1:29" s="6" customFormat="1">
+    <row r="299" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A299" s="7">
         <v>134868</v>
       </c>
@@ -23762,7 +23807,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="300" spans="1:29" s="6" customFormat="1">
+    <row r="300" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A300" s="7">
         <v>134869</v>
       </c>
@@ -23828,7 +23873,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="301" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="301" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A301" s="7">
         <v>134870</v>
       </c>
@@ -23894,7 +23939,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="302" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="302" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A302" s="7">
         <v>134871</v>
       </c>
@@ -23964,7 +24009,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="303" spans="1:29" s="6" customFormat="1">
+    <row r="303" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A303" s="7">
         <v>134872</v>
       </c>
@@ -24032,7 +24077,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="304" spans="1:29" s="6" customFormat="1">
+    <row r="304" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A304" s="7">
         <v>134873</v>
       </c>
@@ -24098,7 +24143,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="305" spans="1:29" s="6" customFormat="1">
+    <row r="305" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A305" s="7">
         <v>134874</v>
       </c>
@@ -24164,7 +24209,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="306" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="306" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A306" s="7">
         <v>134875</v>
       </c>
@@ -24232,7 +24277,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="307" spans="1:29" s="6" customFormat="1">
+    <row r="307" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A307" s="7">
         <v>134876</v>
       </c>
@@ -24300,7 +24345,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="308" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="308" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A308" s="7">
         <v>134877</v>
       </c>
@@ -24370,7 +24415,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="309" spans="1:29" s="6" customFormat="1">
+    <row r="309" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A309" s="7">
         <v>134878</v>
       </c>
@@ -24434,7 +24479,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="310" spans="1:29" s="6" customFormat="1">
+    <row r="310" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A310" s="7">
         <v>134879</v>
       </c>
@@ -24500,7 +24545,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="311" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="311" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A311" s="7">
         <v>134880</v>
       </c>
@@ -24568,7 +24613,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="312" spans="1:29" s="6" customFormat="1">
+    <row r="312" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A312" s="7">
         <v>134881</v>
       </c>
@@ -24632,7 +24677,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="313" spans="1:29" s="6" customFormat="1">
+    <row r="313" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A313" s="7">
         <v>145558</v>
       </c>
@@ -24698,7 +24743,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="314" spans="1:29" s="6" customFormat="1">
+    <row r="314" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A314" s="7">
         <v>134882</v>
       </c>
@@ -24762,7 +24807,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="315" spans="1:29" s="6" customFormat="1">
+    <row r="315" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A315" s="7">
         <v>134883</v>
       </c>
@@ -24826,7 +24871,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="316" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="316" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A316" s="7">
         <v>134884</v>
       </c>
@@ -24896,7 +24941,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="317" spans="1:29" s="6" customFormat="1">
+    <row r="317" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A317" s="7">
         <v>134885</v>
       </c>
@@ -24960,7 +25005,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="318" spans="1:29" s="6" customFormat="1">
+    <row r="318" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A318" s="7">
         <v>134886</v>
       </c>
@@ -25026,7 +25071,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="319" spans="1:29" s="6" customFormat="1">
+    <row r="319" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A319" s="7">
         <v>134887</v>
       </c>
@@ -25090,7 +25135,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="320" spans="1:29" s="6" customFormat="1">
+    <row r="320" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A320" s="7">
         <v>134888</v>
       </c>
@@ -25154,7 +25199,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="321" spans="1:29" s="6" customFormat="1">
+    <row r="321" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A321" s="7">
         <v>134889</v>
       </c>
@@ -25218,7 +25263,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="322" spans="1:29" s="6" customFormat="1">
+    <row r="322" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A322" s="7">
         <v>134890</v>
       </c>
@@ -25286,7 +25331,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="323" spans="1:29" s="6" customFormat="1">
+    <row r="323" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A323" s="7">
         <v>134891</v>
       </c>
@@ -25352,7 +25397,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="324" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="324" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A324" s="7">
         <v>134893</v>
       </c>
@@ -25422,7 +25467,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="325" spans="1:29" s="6" customFormat="1">
+    <row r="325" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A325" s="7">
         <v>134892</v>
       </c>
@@ -25486,7 +25531,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="326" spans="1:29" s="6" customFormat="1">
+    <row r="326" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A326" s="7">
         <v>134894</v>
       </c>
@@ -25550,7 +25595,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="327" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="327" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A327" s="7">
         <v>134895</v>
       </c>
@@ -25620,7 +25665,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="328" spans="1:29" s="6" customFormat="1">
+    <row r="328" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A328" s="7">
         <v>134896</v>
       </c>
@@ -25684,7 +25729,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="329" spans="1:29" s="6" customFormat="1">
+    <row r="329" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A329" s="7">
         <v>134897</v>
       </c>
@@ -25750,7 +25795,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="330" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="330" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A330" s="7">
         <v>134898</v>
       </c>
@@ -25818,7 +25863,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="331" spans="1:29" s="6" customFormat="1">
+    <row r="331" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A331" s="7">
         <v>134899</v>
       </c>
@@ -25882,7 +25927,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="332" spans="1:29" s="6" customFormat="1">
+    <row r="332" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A332" s="7">
         <v>134900</v>
       </c>
@@ -25948,7 +25993,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="333" spans="1:29" s="6" customFormat="1">
+    <row r="333" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A333" s="7">
         <v>134901</v>
       </c>
@@ -26014,7 +26059,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="334" spans="1:29" s="6" customFormat="1">
+    <row r="334" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A334" s="7">
         <v>134902</v>
       </c>
@@ -26082,7 +26127,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="335" spans="1:29" s="6" customFormat="1">
+    <row r="335" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A335" s="7">
         <v>134903</v>
       </c>
@@ -26148,7 +26193,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="336" spans="1:29" s="6" customFormat="1">
+    <row r="336" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A336" s="7">
         <v>134904</v>
       </c>
@@ -26212,7 +26257,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="337" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="337" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A337" s="7">
         <v>134905</v>
       </c>
@@ -26280,7 +26325,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="338" spans="1:29" s="6" customFormat="1">
+    <row r="338" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A338" s="7">
         <v>134906</v>
       </c>
@@ -26346,7 +26391,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="339" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="339" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A339" s="7">
         <v>134907</v>
       </c>
@@ -26412,7 +26457,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="340" spans="1:29" s="6" customFormat="1">
+    <row r="340" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A340" s="7">
         <v>134908</v>
       </c>
@@ -26480,7 +26525,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="341" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="341" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A341" s="7">
         <v>134909</v>
       </c>
@@ -26546,7 +26591,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="342" spans="1:29" s="6" customFormat="1">
+    <row r="342" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A342" s="7">
         <v>134910</v>
       </c>
@@ -26612,7 +26657,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="343" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="343" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A343" s="7">
         <v>134912</v>
       </c>
@@ -26680,7 +26725,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="344" spans="1:29" s="6" customFormat="1">
+    <row r="344" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A344" s="7">
         <v>134911</v>
       </c>
@@ -26744,7 +26789,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="345" spans="1:29" s="6" customFormat="1">
+    <row r="345" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A345" s="7">
         <v>134913</v>
       </c>
@@ -26810,7 +26855,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="346" spans="1:29" s="6" customFormat="1">
+    <row r="346" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A346" s="7">
         <v>134914</v>
       </c>
@@ -26878,7 +26923,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="347" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="347" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A347" s="7">
         <v>134915</v>
       </c>
@@ -26948,7 +26993,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="348" spans="1:29" s="6" customFormat="1">
+    <row r="348" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A348" s="7">
         <v>134916</v>
       </c>
@@ -27014,7 +27059,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="349" spans="1:29" s="6" customFormat="1">
+    <row r="349" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A349" s="7">
         <v>134917</v>
       </c>
@@ -27082,7 +27127,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="350" spans="1:29" s="6" customFormat="1">
+    <row r="350" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A350" s="7">
         <v>134918</v>
       </c>
@@ -27148,7 +27193,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="351" spans="1:29" s="6" customFormat="1">
+    <row r="351" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A351" s="7">
         <v>134919</v>
       </c>
@@ -27214,7 +27259,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="352" spans="1:29" s="6" customFormat="1">
+    <row r="352" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A352" s="7">
         <v>134920</v>
       </c>
@@ -27280,7 +27325,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="353" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="353" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A353" s="7">
         <v>134921</v>
       </c>
@@ -27348,7 +27393,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="354" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="354" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A354" s="7">
         <v>134922</v>
       </c>
@@ -27418,7 +27463,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="355" spans="1:29" s="6" customFormat="1">
+    <row r="355" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A355" s="7">
         <v>134923</v>
       </c>
@@ -27486,7 +27531,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="356" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="356" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A356" s="7">
         <v>134924</v>
       </c>
@@ -27556,7 +27601,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="357" spans="1:29" s="6" customFormat="1">
+    <row r="357" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A357" s="7">
         <v>134925</v>
       </c>
@@ -27620,7 +27665,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="358" spans="1:29" s="6" customFormat="1">
+    <row r="358" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A358" s="7">
         <v>134926</v>
       </c>
@@ -27684,7 +27729,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="359" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="359" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A359" s="7">
         <v>145559</v>
       </c>
@@ -27750,7 +27795,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="360" spans="1:29" s="6" customFormat="1">
+    <row r="360" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A360" s="7">
         <v>134927</v>
       </c>
@@ -27816,7 +27861,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="361" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="361" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A361" s="7">
         <v>134928</v>
       </c>
@@ -27884,7 +27929,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="362" spans="1:29" s="6" customFormat="1">
+    <row r="362" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A362" s="7">
         <v>134929</v>
       </c>
@@ -27948,7 +27993,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="363" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="363" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A363" s="7">
         <v>134930</v>
       </c>
@@ -28014,7 +28059,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="364" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="364" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A364" s="7">
         <v>134931</v>
       </c>
@@ -28080,7 +28125,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="365" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="365" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A365" s="7">
         <v>134932</v>
       </c>
@@ -28150,7 +28195,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="366" spans="1:29" s="6" customFormat="1">
+    <row r="366" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A366" s="7">
         <v>134933</v>
       </c>
@@ -28216,7 +28261,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="367" spans="1:29" s="6" customFormat="1">
+    <row r="367" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A367" s="7">
         <v>134934</v>
       </c>
@@ -28282,7 +28327,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="368" spans="1:29" s="6" customFormat="1">
+    <row r="368" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A368" s="7">
         <v>134935</v>
       </c>
@@ -28348,7 +28393,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="369" spans="1:29" s="6" customFormat="1">
+    <row r="369" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A369" s="7">
         <v>134936</v>
       </c>
@@ -28414,7 +28459,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="370" spans="1:29" s="6" customFormat="1">
+    <row r="370" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A370" s="7">
         <v>134937</v>
       </c>
@@ -28482,7 +28527,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="371" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="371" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A371" s="7">
         <v>134938</v>
       </c>
@@ -28550,7 +28595,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="372" spans="1:29" s="6" customFormat="1">
+    <row r="372" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A372" s="7">
         <v>134939</v>
       </c>
@@ -28616,7 +28661,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="373" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="373" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A373" s="7">
         <v>134940</v>
       </c>
@@ -28686,7 +28731,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="374" spans="1:29" s="6" customFormat="1">
+    <row r="374" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A374" s="7">
         <v>134941</v>
       </c>
@@ -28754,7 +28799,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="375" spans="1:29" s="6" customFormat="1">
+    <row r="375" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A375" s="7">
         <v>134942</v>
       </c>
@@ -28820,7 +28865,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="376" spans="1:29" s="6" customFormat="1">
+    <row r="376" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A376" s="7">
         <v>134943</v>
       </c>
@@ -28886,7 +28931,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="377" spans="1:29" s="6" customFormat="1">
+    <row r="377" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A377" s="7">
         <v>145560</v>
       </c>
@@ -28952,7 +28997,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="378" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="378" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A378" s="7">
         <v>134944</v>
       </c>
@@ -29020,7 +29065,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="379" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="379" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A379" s="7">
         <v>134945</v>
       </c>
@@ -29088,7 +29133,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="380" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="380" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A380" s="7">
         <v>134946</v>
       </c>
@@ -29154,7 +29199,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="381" spans="1:29" s="6" customFormat="1">
+    <row r="381" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A381" s="7">
         <v>134947</v>
       </c>
@@ -29220,7 +29265,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="382" spans="1:29" s="6" customFormat="1">
+    <row r="382" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A382" s="7">
         <v>134948</v>
       </c>
@@ -29288,7 +29333,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="383" spans="1:29" s="6" customFormat="1">
+    <row r="383" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A383" s="7">
         <v>134949</v>
       </c>
@@ -29352,7 +29397,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="384" spans="1:29" s="6" customFormat="1">
+    <row r="384" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A384" s="7">
         <v>134950</v>
       </c>
@@ -29418,7 +29463,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="385" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="385" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A385" s="7">
         <v>134951</v>
       </c>
@@ -29484,7 +29529,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="386" spans="1:29" s="6" customFormat="1">
+    <row r="386" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A386" s="7">
         <v>134952</v>
       </c>
@@ -29550,7 +29595,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="387" spans="1:29" s="6" customFormat="1">
+    <row r="387" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A387" s="7">
         <v>134953</v>
       </c>
@@ -29618,7 +29663,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="388" spans="1:29" s="6" customFormat="1">
+    <row r="388" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A388" s="7">
         <v>134954</v>
       </c>
@@ -29684,7 +29729,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="389" spans="1:29" s="6" customFormat="1">
+    <row r="389" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A389" s="7">
         <v>134955</v>
       </c>
@@ -29746,7 +29791,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="390" spans="1:29" s="6" customFormat="1">
+    <row r="390" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A390" s="7">
         <v>134956</v>
       </c>
@@ -29812,7 +29857,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="391" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="391" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A391" s="7">
         <v>134957</v>
       </c>
@@ -29878,7 +29923,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="392" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="392" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A392" s="7">
         <v>134958</v>
       </c>
@@ -29948,7 +29993,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="393" spans="1:29" s="6" customFormat="1">
+    <row r="393" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A393" s="7">
         <v>134959</v>
       </c>
@@ -30014,7 +30059,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="394" spans="1:29" s="6" customFormat="1">
+    <row r="394" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A394" s="7">
         <v>134960</v>
       </c>
@@ -30078,7 +30123,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="395" spans="1:29" s="6" customFormat="1">
+    <row r="395" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A395" s="7">
         <v>134961</v>
       </c>
@@ -30146,7 +30191,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="396" spans="1:29" s="6" customFormat="1">
+    <row r="396" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A396" s="7">
         <v>134962</v>
       </c>
@@ -30214,7 +30259,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="397" spans="1:29" s="6" customFormat="1">
+    <row r="397" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A397" s="7">
         <v>134963</v>
       </c>
@@ -30278,7 +30323,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="398" spans="1:29" s="6" customFormat="1">
+    <row r="398" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A398" s="7">
         <v>134964</v>
       </c>
@@ -30342,7 +30387,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="399" spans="1:29" s="6" customFormat="1">
+    <row r="399" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A399" s="7">
         <v>134965</v>
       </c>
@@ -30408,7 +30453,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="400" spans="1:29" s="6" customFormat="1">
+    <row r="400" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A400" s="7">
         <v>134966</v>
       </c>
@@ -30476,7 +30521,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="401" spans="1:29" s="6" customFormat="1">
+    <row r="401" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A401" s="7">
         <v>134967</v>
       </c>
@@ -30542,7 +30587,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="402" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="402" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A402" s="7">
         <v>134968</v>
       </c>
@@ -30610,7 +30655,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="403" spans="1:29" s="6" customFormat="1">
+    <row r="403" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A403" s="7">
         <v>134969</v>
       </c>
@@ -30676,7 +30721,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="404" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="404" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A404" s="7">
         <v>134970</v>
       </c>
@@ -30746,7 +30791,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="405" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="405" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A405" s="7">
         <v>134971</v>
       </c>
@@ -30814,7 +30859,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="406" spans="1:29" s="6" customFormat="1">
+    <row r="406" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A406" s="7">
         <v>134972</v>
       </c>
@@ -30880,7 +30925,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="407" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="407" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A407" s="7">
         <v>134974</v>
       </c>
@@ -30950,7 +30995,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="408" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="408" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A408" s="7">
         <v>134973</v>
       </c>
@@ -31018,7 +31063,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="409" spans="1:29" s="6" customFormat="1">
+    <row r="409" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A409" s="7">
         <v>134975</v>
       </c>
@@ -31082,7 +31127,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="410" spans="1:29" s="6" customFormat="1">
+    <row r="410" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A410" s="7">
         <v>134976</v>
       </c>
@@ -31150,7 +31195,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="411" spans="1:29" s="6" customFormat="1">
+    <row r="411" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A411" s="7">
         <v>134977</v>
       </c>
@@ -31214,7 +31259,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="412" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="412" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A412" s="7">
         <v>134978</v>
       </c>
@@ -31284,7 +31329,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="413" spans="1:29" s="6" customFormat="1">
+    <row r="413" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A413" s="7">
         <v>134979</v>
       </c>
@@ -31350,7 +31395,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="414" spans="1:29" s="6" customFormat="1">
+    <row r="414" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A414" s="7">
         <v>134980</v>
       </c>
@@ -31416,7 +31461,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="415" spans="1:29" s="6" customFormat="1">
+    <row r="415" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A415" s="7">
         <v>134981</v>
       </c>
@@ -31484,7 +31529,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="416" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="416" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A416" s="7">
         <v>134982</v>
       </c>
@@ -31554,7 +31599,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="417" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="417" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A417" s="7">
         <v>134983</v>
       </c>
@@ -31622,7 +31667,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="418" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="418" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A418" s="7">
         <v>134984</v>
       </c>
@@ -31690,7 +31735,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="419" spans="1:29" s="6" customFormat="1">
+    <row r="419" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A419" s="7">
         <v>134985</v>
       </c>
@@ -31754,7 +31799,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="420" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="420" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A420" s="7">
         <v>134986</v>
       </c>
@@ -31822,7 +31867,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="421" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="421" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A421" s="7">
         <v>134987</v>
       </c>
@@ -31890,7 +31935,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="422" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="422" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A422" s="7">
         <v>134988</v>
       </c>
@@ -31956,7 +32001,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="423" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="423" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A423" s="7">
         <v>134989</v>
       </c>
@@ -32024,7 +32069,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="424" spans="1:29" s="6" customFormat="1">
+    <row r="424" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A424" s="7">
         <v>134990</v>
       </c>
@@ -32092,7 +32137,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="425" spans="1:29" s="6" customFormat="1">
+    <row r="425" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A425" s="7">
         <v>134991</v>
       </c>
@@ -32156,7 +32201,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="426" spans="1:29" s="6" customFormat="1">
+    <row r="426" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A426" s="7">
         <v>134992</v>
       </c>
@@ -32222,7 +32267,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="427" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="427" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A427" s="7">
         <v>134993</v>
       </c>
@@ -32292,7 +32337,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="428" spans="1:29" s="6" customFormat="1">
+    <row r="428" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A428" s="7">
         <v>134994</v>
       </c>
@@ -32358,7 +32403,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="429" spans="1:29" s="6" customFormat="1">
+    <row r="429" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A429" s="7">
         <v>134995</v>
       </c>
@@ -32422,7 +32467,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="430" spans="1:29" s="6" customFormat="1">
+    <row r="430" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A430" s="7">
         <v>134996</v>
       </c>
@@ -32488,7 +32533,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="431" spans="1:29" s="6" customFormat="1">
+    <row r="431" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A431" s="7">
         <v>134997</v>
       </c>
@@ -32554,7 +32599,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="432" spans="1:29" s="6" customFormat="1">
+    <row r="432" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A432" s="7">
         <v>134998</v>
       </c>
@@ -32618,7 +32663,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="433" spans="1:29" s="6" customFormat="1">
+    <row r="433" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A433" s="7">
         <v>134999</v>
       </c>
@@ -32682,7 +32727,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="434" spans="1:29" s="6" customFormat="1">
+    <row r="434" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A434" s="7">
         <v>135000</v>
       </c>
@@ -32748,7 +32793,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="435" spans="1:29" s="6" customFormat="1">
+    <row r="435" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A435" s="7">
         <v>135001</v>
       </c>
@@ -32812,7 +32857,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="436" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="436" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A436" s="7">
         <v>135002</v>
       </c>
@@ -32880,7 +32925,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="437" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="437" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A437" s="7">
         <v>135003</v>
       </c>
@@ -32948,7 +32993,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="438" spans="1:29" s="6" customFormat="1">
+    <row r="438" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A438" s="7">
         <v>135004</v>
       </c>
@@ -33016,7 +33061,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="439" spans="1:29" s="6" customFormat="1">
+    <row r="439" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A439" s="7">
         <v>135005</v>
       </c>
@@ -33080,7 +33125,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="440" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="440" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A440" s="7">
         <v>135006</v>
       </c>
@@ -33148,7 +33193,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="441" spans="1:29" s="6" customFormat="1">
+    <row r="441" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A441" s="7">
         <v>135007</v>
       </c>
@@ -33214,7 +33259,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="442" spans="1:29" s="6" customFormat="1" ht="26.25">
+    <row r="442" spans="1:29" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.3">
       <c r="A442" s="7">
         <v>135008</v>
       </c>
@@ -33282,7 +33327,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="443" spans="1:29" s="6" customFormat="1">
+    <row r="443" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A443" s="7">
         <v>145561</v>
       </c>
@@ -33346,7 +33391,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="444" spans="1:29" s="6" customFormat="1">
+    <row r="444" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A444" s="7">
         <v>135009</v>
       </c>
@@ -33414,13 +33459,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N444">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N444" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>ПрЗахоронения</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L444">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L444" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>ПрСмерти</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S444">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S444" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>Районы</formula1>
     </dataValidation>
   </dataValidations>
@@ -33430,12 +33475,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
@@ -33443,12 +33488,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>